<commit_message>
Percy 2017-8-11 Add Tax Registration No.
</commit_message>
<xml_diff>
--- a/dr/protected/commands/template/m_template.xlsx
+++ b/dr/protected/commands/template/m_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3947,9 +3947,9 @@
     <cellStyle name="60% - 輔色4" xfId="16"/>
     <cellStyle name="60% - 輔色5" xfId="17"/>
     <cellStyle name="60% - 輔色6" xfId="18"/>
-    <cellStyle name="Comma" xfId="28" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="29"/>
+    <cellStyle name="千分位" xfId="28" builtinId="3"/>
     <cellStyle name="合計" xfId="26"/>
     <cellStyle name="連結的儲存格" xfId="27"/>
     <cellStyle name="備註" xfId="19"/>
@@ -4689,7 +4689,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5012,7 +5012,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6404,7 +6404,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -7518,7 +7518,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -8910,7 +8910,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -10024,7 +10024,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -11416,7 +11416,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -12530,7 +12530,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -13922,7 +13922,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -15036,7 +15036,7 @@
   <dimension ref="A1:E246"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -17144,7 +17144,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -18535,8 +18535,8 @@
       <c r="D108" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="E108" s="129">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+      <c r="E108" s="73">
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -19650,7 +19650,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -21042,7 +21042,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="136"/>
@@ -22156,7 +22156,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -23548,7 +23548,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -24662,7 +24662,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -26054,7 +26054,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -27168,7 +27168,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -28559,8 +28559,8 @@
       <c r="D108" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="E108" s="129">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+      <c r="E108" s="73">
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -29674,7 +29674,7 @@
   <dimension ref="A1:I246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -31067,7 +31067,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -32181,7 +32181,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -33573,7 +33573,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -34658,11 +34658,9 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="17">
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A107:A109"/>
     <mergeCell ref="A126:F126"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A119:A122"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C73:E73"/>
@@ -34673,8 +34671,10 @@
     <mergeCell ref="A92:A93"/>
     <mergeCell ref="A95:A96"/>
     <mergeCell ref="A110:A114"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A119:A122"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A107:A109"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34690,7 +34690,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -36082,7 +36082,7 @@
         <v>145</v>
       </c>
       <c r="E108" s="73">
-        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;0,0,1)))</f>
+        <f>IF(C108&gt;0.2,3,IF(C108&gt;0.1,5,IF(C108&gt;=0,1,0)))</f>
         <v>1</v>
       </c>
       <c r="F108" s="72"/>
@@ -37167,10 +37167,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="17">
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="A110:A114"/>
-    <mergeCell ref="A117:A118"/>
     <mergeCell ref="A125:F125"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
@@ -37184,6 +37180,10 @@
     <mergeCell ref="A119:A122"/>
     <mergeCell ref="A97:A98"/>
     <mergeCell ref="A102:A104"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A110:A114"/>
+    <mergeCell ref="A117:A118"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>